<commit_message>
excel test suite update
-Added test suite functionality to excel sheet
-adjusted file path constants to work correctly when installed on a new
device
-small changes to log to improve appearance
</commit_message>
<xml_diff>
--- a/bgdSelFramework/bin/dataEngine/DataEngine.xlsx
+++ b/bgdSelFramework/bin/dataEngine/DataEngine.xlsx
@@ -4,13 +4,15 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16635" windowHeight="3765" tabRatio="575" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="21405" windowHeight="7110" tabRatio="575" activeTab="3"/>
   </bookViews>
   <sheets>
-    <sheet name="Test Cases" sheetId="2" r:id="rId1"/>
-    <sheet name="Test Steps" sheetId="1" r:id="rId2"/>
-    <sheet name="Test Data" sheetId="3" r:id="rId3"/>
-    <sheet name="Settings" sheetId="4" r:id="rId4"/>
+    <sheet name="Execution" sheetId="9" r:id="rId1"/>
+    <sheet name="Test Suites" sheetId="10" r:id="rId2"/>
+    <sheet name="Test Cases" sheetId="2" r:id="rId3"/>
+    <sheet name="Test Steps" sheetId="1" r:id="rId4"/>
+    <sheet name="Test Data" sheetId="3" r:id="rId5"/>
+    <sheet name="Settings" sheetId="4" r:id="rId6"/>
   </sheets>
   <definedNames>
     <definedName name="action_keywords">Settings!$AB$2:$AB$11</definedName>
@@ -32,6 +34,7 @@
     <definedName name="searchResults_diamond">Settings!$Q$2:$Q$13</definedName>
     <definedName name="searchResults_setting">Settings!$P$2:$P$9</definedName>
     <definedName name="shopping_cart">Settings!$V$2:$V$6</definedName>
+    <definedName name="testCases">'Test Cases'!$A$2:$A$15</definedName>
     <definedName name="top_nav_customDesign">Settings!$E$2:$E$17</definedName>
     <definedName name="top_nav_designers">Settings!$I$2:$I$15</definedName>
     <definedName name="top_nav_diamonds">Settings!$D$2:$D$27</definedName>
@@ -43,12 +46,12 @@
     <definedName name="top_navigation">Settings!$B$2:$B$18</definedName>
   </definedNames>
   <calcPr calcId="0"/>
-  <oleSize ref="A7:D16"/>
+  <oleSize ref="A1:F20"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="806" uniqueCount="493">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="792" uniqueCount="499">
   <si>
     <t>Description</t>
   </si>
@@ -1526,7 +1529,25 @@
     <t>Click the "Continue" button</t>
   </si>
   <si>
-    <t>PASS</t>
+    <t>smokeTest_01</t>
+  </si>
+  <si>
+    <t>Test Suite ID</t>
+  </si>
+  <si>
+    <t>Clear browser cache</t>
+  </si>
+  <si>
+    <t>smokeTest_02</t>
+  </si>
+  <si>
+    <t>Build a ring with the workbench and complete the checkout process</t>
+  </si>
+  <si>
+    <t>Example additional suite</t>
+  </si>
+  <si>
+    <t>No</t>
   </si>
 </sst>
 </file>
@@ -1583,7 +1604,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="62">
+  <borders count="66">
     <border>
       <left/>
       <right/>
@@ -2492,12 +2513,72 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="73">
+  <cellXfs count="77">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -2581,6 +2662,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="59" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="60" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="61" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="62" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="63" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="64" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="65" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="20% - Accent3" xfId="1" builtinId="38"/>
@@ -2886,10 +2971,247 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D19"/>
+  <dimension ref="A1:D5"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="D14" sqref="D2:D14"/>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <selection activeCell="D2" sqref="D2:D4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="25" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="79.42578125" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="9.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="12" customWidth="1" collapsed="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" s="8" t="s">
+        <v>493</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>455</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D2" s="65"/>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>492</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>496</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D3" s="76"/>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>450</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>494</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D4" s="63"/>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>495</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>497</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>498</v>
+      </c>
+      <c r="D5" s="24"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D12"/>
+  <sheetViews>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <selection activeCell="D3" sqref="D3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="2" width="12.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="10.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="34.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="C1" s="8" t="s">
+        <v>450</v>
+      </c>
+      <c r="D1" s="8" t="s">
+        <v>492</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>450</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>454</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>403</v>
+      </c>
+      <c r="B3" s="1"/>
+      <c r="C3" s="1"/>
+      <c r="D3" s="1" t="s">
+        <v>381</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>403</v>
+      </c>
+      <c r="B4" s="1"/>
+      <c r="C4" s="1"/>
+      <c r="D4" s="1" t="s">
+        <v>460</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>403</v>
+      </c>
+      <c r="B5" s="1"/>
+      <c r="C5" s="1"/>
+      <c r="D5" s="1" t="s">
+        <v>461</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
+        <v>403</v>
+      </c>
+      <c r="B6" s="1"/>
+      <c r="C6" s="1"/>
+      <c r="D6" s="1" t="s">
+        <v>464</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
+        <v>403</v>
+      </c>
+      <c r="B7" s="1"/>
+      <c r="C7" s="1"/>
+      <c r="D7" s="1" t="s">
+        <v>462</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
+        <v>403</v>
+      </c>
+      <c r="B8" s="1"/>
+      <c r="C8" s="1"/>
+      <c r="D8" s="1" t="s">
+        <v>463</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
+        <v>403</v>
+      </c>
+      <c r="B9" s="1"/>
+      <c r="C9" s="1"/>
+      <c r="D9" s="1" t="s">
+        <v>465</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" s="1" t="s">
+        <v>403</v>
+      </c>
+      <c r="B10" s="1"/>
+      <c r="C10" s="1"/>
+      <c r="D10" s="1" t="s">
+        <v>419</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" s="1" t="s">
+        <v>403</v>
+      </c>
+      <c r="B11" s="1"/>
+      <c r="C11" s="1"/>
+      <c r="D11" s="1" t="s">
+        <v>459</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" s="1" t="s">
+        <v>403</v>
+      </c>
+      <c r="B12" s="1"/>
+      <c r="C12" s="1"/>
+      <c r="D12" s="1" t="s">
+        <v>458</v>
+      </c>
+    </row>
+  </sheetData>
+  <dataValidations count="1">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:D12 A2:C2">
+      <formula1>testCases</formula1>
+    </dataValidation>
+  </dataValidations>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D27"/>
+  <sheetViews>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2906,10 +3228,7 @@
       <c r="B1" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="8" t="s">
-        <v>6</v>
-      </c>
-      <c r="D1" s="4" t="s">
+      <c r="C1" s="4" t="s">
         <v>15</v>
       </c>
     </row>
@@ -2920,12 +3239,7 @@
       <c r="B2" s="1" t="s">
         <v>455</v>
       </c>
-      <c r="C2" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="D2" s="22" t="s">
-        <v>492</v>
-      </c>
+      <c r="C2" s="21"/>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
@@ -2934,12 +3248,7 @@
       <c r="B3" s="1" t="s">
         <v>457</v>
       </c>
-      <c r="C3" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="D3" s="24" t="s">
-        <v>492</v>
-      </c>
+      <c r="C3" s="22"/>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
@@ -2948,12 +3257,7 @@
       <c r="B4" s="1" t="s">
         <v>386</v>
       </c>
-      <c r="C4" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="D4" s="27" t="s">
-        <v>492</v>
-      </c>
+      <c r="C4" s="23"/>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
@@ -2962,12 +3266,7 @@
       <c r="B5" s="1" t="s">
         <v>466</v>
       </c>
-      <c r="C5" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="D5" s="30" t="s">
-        <v>492</v>
-      </c>
+      <c r="C5" s="24"/>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
@@ -2976,12 +3275,7 @@
       <c r="B6" s="1" t="s">
         <v>468</v>
       </c>
-      <c r="C6" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="D6" s="33" t="s">
-        <v>492</v>
-      </c>
+      <c r="C6" s="25"/>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
@@ -2990,12 +3284,7 @@
       <c r="B7" s="1" t="s">
         <v>467</v>
       </c>
-      <c r="C7" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="D7" s="36" t="s">
-        <v>492</v>
-      </c>
+      <c r="C7" s="26"/>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
@@ -3004,12 +3293,7 @@
       <c r="B8" s="1" t="s">
         <v>470</v>
       </c>
-      <c r="C8" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="D8" s="41" t="s">
-        <v>492</v>
-      </c>
+      <c r="C8" s="27"/>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
@@ -3018,12 +3302,7 @@
       <c r="B9" s="1" t="s">
         <v>469</v>
       </c>
-      <c r="C9" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="D9" s="43" t="s">
-        <v>492</v>
-      </c>
+      <c r="C9" s="28"/>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
@@ -3032,12 +3311,7 @@
       <c r="B10" s="1" t="s">
         <v>471</v>
       </c>
-      <c r="C10" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="D10" s="45" t="s">
-        <v>492</v>
-      </c>
+      <c r="C10" s="29"/>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
@@ -3046,12 +3320,7 @@
       <c r="B11" s="1" t="s">
         <v>449</v>
       </c>
-      <c r="C11" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="D11" s="48" t="s">
-        <v>492</v>
-      </c>
+      <c r="C11" s="30"/>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
@@ -3060,12 +3329,7 @@
       <c r="B12" s="1" t="s">
         <v>472</v>
       </c>
-      <c r="C12" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="D12" s="62" t="s">
-        <v>492</v>
-      </c>
+      <c r="C12" s="31"/>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
@@ -3074,12 +3338,7 @@
       <c r="B13" s="1" t="s">
         <v>473</v>
       </c>
-      <c r="C13" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="D13" s="70" t="s">
-        <v>492</v>
-      </c>
+      <c r="C13" s="32"/>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
@@ -3088,30 +3347,41 @@
       <c r="B14" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="C14" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="D14" s="72" t="s">
-        <v>492</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25"/>
+      <c r="C14" s="34"/>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15" s="1" t="s">
+        <v>450</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>494</v>
+      </c>
+      <c r="C15" s="34"/>
+    </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25"/>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25"/>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25"/>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25"/>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25"/>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25"/>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25"/>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25"/>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25"/>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25"/>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25"/>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I43"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="H2" sqref="H2:H40"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="H2" sqref="H2:H41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3173,9 +3443,7 @@
       <c r="G2" s="17" t="s">
         <v>382</v>
       </c>
-      <c r="H2" s="21" t="s">
-        <v>492</v>
-      </c>
+      <c r="H2" s="64"/>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="10" t="s">
@@ -3197,9 +3465,7 @@
       <c r="G3" t="s">
         <v>456</v>
       </c>
-      <c r="H3" s="23" t="s">
-        <v>492</v>
-      </c>
+      <c r="H3" s="66"/>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="17" t="s">
@@ -3221,9 +3487,7 @@
       <c r="G4" s="17" t="s">
         <v>403</v>
       </c>
-      <c r="H4" s="25" t="s">
-        <v>492</v>
-      </c>
+      <c r="H4" s="67"/>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="17" t="s">
@@ -3247,9 +3511,7 @@
       <c r="G5" s="17" t="s">
         <v>403</v>
       </c>
-      <c r="H5" s="26" t="s">
-        <v>492</v>
-      </c>
+      <c r="H5" s="68"/>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="10" t="s">
@@ -3273,9 +3535,7 @@
       <c r="G6" s="6" t="s">
         <v>403</v>
       </c>
-      <c r="H6" s="28" t="s">
-        <v>492</v>
-      </c>
+      <c r="H6" s="69"/>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="10" t="s">
@@ -3299,9 +3559,7 @@
       <c r="G7" s="6" t="s">
         <v>403</v>
       </c>
-      <c r="H7" s="29" t="s">
-        <v>492</v>
-      </c>
+      <c r="H7" s="70"/>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="17" t="s">
@@ -3325,9 +3583,7 @@
       <c r="G8" s="17" t="s">
         <v>403</v>
       </c>
-      <c r="H8" s="31" t="s">
-        <v>492</v>
-      </c>
+      <c r="H8" s="71"/>
     </row>
     <row r="9" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="17" t="s">
@@ -3351,9 +3607,7 @@
       <c r="G9" s="17" t="s">
         <v>403</v>
       </c>
-      <c r="H9" s="32" t="s">
-        <v>492</v>
-      </c>
+      <c r="H9" s="72"/>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" s="10" t="s">
@@ -3377,9 +3631,7 @@
       <c r="G10" s="6" t="s">
         <v>404</v>
       </c>
-      <c r="H10" s="34" t="s">
-        <v>492</v>
-      </c>
+      <c r="H10" s="73"/>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" s="10" t="s">
@@ -3403,9 +3655,7 @@
       <c r="G11" s="11" t="s">
         <v>403</v>
       </c>
-      <c r="H11" s="35" t="s">
-        <v>492</v>
-      </c>
+      <c r="H11" s="74"/>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" s="17" t="s">
@@ -3429,9 +3679,7 @@
       <c r="G12" s="17" t="s">
         <v>403</v>
       </c>
-      <c r="H12" s="37" t="s">
-        <v>492</v>
-      </c>
+      <c r="H12" s="75"/>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" s="17" t="s">
@@ -3455,9 +3703,7 @@
       <c r="G13" s="17" t="s">
         <v>403</v>
       </c>
-      <c r="H13" s="38" t="s">
-        <v>492</v>
-      </c>
+      <c r="H13" s="35"/>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" s="17" t="s">
@@ -3481,9 +3727,7 @@
       <c r="G14" s="17" t="s">
         <v>403</v>
       </c>
-      <c r="H14" s="39" t="s">
-        <v>492</v>
-      </c>
+      <c r="H14" s="36"/>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" s="17" t="s">
@@ -3507,9 +3751,7 @@
       <c r="G15" s="17" t="s">
         <v>403</v>
       </c>
-      <c r="H15" s="40" t="s">
-        <v>492</v>
-      </c>
+      <c r="H15" s="37"/>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" s="10" t="s">
@@ -3533,9 +3775,7 @@
       <c r="G16" s="10" t="s">
         <v>403</v>
       </c>
-      <c r="H16" s="42" t="s">
-        <v>492</v>
-      </c>
+      <c r="H16" s="38"/>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" s="17" t="s">
@@ -3559,9 +3799,7 @@
       <c r="G17" s="17" t="s">
         <v>403</v>
       </c>
-      <c r="H17" s="44" t="s">
-        <v>492</v>
-      </c>
+      <c r="H17" s="39"/>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18" s="10" t="s">
@@ -3585,9 +3823,7 @@
       <c r="G18" s="10" t="s">
         <v>403</v>
       </c>
-      <c r="H18" s="46" t="s">
-        <v>492</v>
-      </c>
+      <c r="H18" s="40"/>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" s="10" t="s">
@@ -3611,9 +3847,7 @@
       <c r="G19" s="10" t="s">
         <v>403</v>
       </c>
-      <c r="H19" s="47" t="s">
-        <v>492</v>
-      </c>
+      <c r="H19" s="41"/>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20" s="17" t="s">
@@ -3637,9 +3871,7 @@
       <c r="G20" s="17" t="s">
         <v>433</v>
       </c>
-      <c r="H20" s="49" t="s">
-        <v>492</v>
-      </c>
+      <c r="H20" s="42"/>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21" s="17" t="s">
@@ -3663,9 +3895,7 @@
       <c r="G21" s="17" t="s">
         <v>434</v>
       </c>
-      <c r="H21" s="50" t="s">
-        <v>492</v>
-      </c>
+      <c r="H21" s="43"/>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22" s="17" t="s">
@@ -3689,9 +3919,7 @@
       <c r="G22" s="17" t="s">
         <v>435</v>
       </c>
-      <c r="H22" s="51" t="s">
-        <v>492</v>
-      </c>
+      <c r="H22" s="44"/>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23" s="17" t="s">
@@ -3715,9 +3943,7 @@
       <c r="G23" s="17" t="s">
         <v>436</v>
       </c>
-      <c r="H23" s="52" t="s">
-        <v>492</v>
-      </c>
+      <c r="H23" s="45"/>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A24" s="17" t="s">
@@ -3741,9 +3967,7 @@
       <c r="G24" s="17" t="s">
         <v>437</v>
       </c>
-      <c r="H24" s="53" t="s">
-        <v>492</v>
-      </c>
+      <c r="H24" s="46"/>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A25" s="17" t="s">
@@ -3767,9 +3991,7 @@
       <c r="G25" s="17" t="s">
         <v>438</v>
       </c>
-      <c r="H25" s="54" t="s">
-        <v>492</v>
-      </c>
+      <c r="H25" s="47"/>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A26" s="17" t="s">
@@ -3793,9 +4015,7 @@
       <c r="G26" s="17" t="s">
         <v>484</v>
       </c>
-      <c r="H26" s="55" t="s">
-        <v>492</v>
-      </c>
+      <c r="H26" s="48"/>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A27" s="17" t="s">
@@ -3819,9 +4039,7 @@
       <c r="G27" s="17" t="s">
         <v>439</v>
       </c>
-      <c r="H27" s="56" t="s">
-        <v>492</v>
-      </c>
+      <c r="H27" s="49"/>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A28" s="17" t="s">
@@ -3845,9 +4063,7 @@
       <c r="G28" s="17" t="s">
         <v>440</v>
       </c>
-      <c r="H28" s="57" t="s">
-        <v>492</v>
-      </c>
+      <c r="H28" s="50"/>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A29" s="17" t="s">
@@ -3871,9 +4087,7 @@
       <c r="G29" s="17" t="s">
         <v>440</v>
       </c>
-      <c r="H29" s="58" t="s">
-        <v>492</v>
-      </c>
+      <c r="H29" s="51"/>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A30" s="17" t="s">
@@ -3895,9 +4109,7 @@
       <c r="G30" s="17" t="s">
         <v>403</v>
       </c>
-      <c r="H30" s="59" t="s">
-        <v>492</v>
-      </c>
+      <c r="H30" s="52"/>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A31" s="17" t="s">
@@ -3921,9 +4133,7 @@
       <c r="G31" s="17" t="s">
         <v>441</v>
       </c>
-      <c r="H31" s="60" t="s">
-        <v>492</v>
-      </c>
+      <c r="H31" s="53"/>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A32" s="17" t="s">
@@ -3947,9 +4157,7 @@
       <c r="G32" s="17" t="s">
         <v>403</v>
       </c>
-      <c r="H32" s="61" t="s">
-        <v>492</v>
-      </c>
+      <c r="H32" s="54"/>
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A33" s="9" t="s">
@@ -3973,9 +4181,7 @@
       <c r="G33" s="10" t="s">
         <v>485</v>
       </c>
-      <c r="H33" s="63" t="s">
-        <v>492</v>
-      </c>
+      <c r="H33" s="55"/>
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A34" s="9" t="s">
@@ -3999,9 +4205,7 @@
       <c r="G34" t="s">
         <v>452</v>
       </c>
-      <c r="H34" s="64" t="s">
-        <v>492</v>
-      </c>
+      <c r="H34" s="56"/>
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A35" s="9" t="s">
@@ -4025,9 +4229,7 @@
       <c r="G35" s="10" t="s">
         <v>451</v>
       </c>
-      <c r="H35" s="65" t="s">
-        <v>492</v>
-      </c>
+      <c r="H35" s="57"/>
     </row>
     <row r="36" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A36" s="9" t="s">
@@ -4051,9 +4253,7 @@
       <c r="G36" s="10" t="s">
         <v>486</v>
       </c>
-      <c r="H36" s="66" t="s">
-        <v>492</v>
-      </c>
+      <c r="H36" s="58"/>
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A37" s="9" t="s">
@@ -4077,9 +4277,7 @@
       <c r="G37" s="10" t="s">
         <v>487</v>
       </c>
-      <c r="H37" s="67" t="s">
-        <v>492</v>
-      </c>
+      <c r="H37" s="59"/>
     </row>
     <row r="38" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A38" s="9" t="s">
@@ -4103,9 +4301,7 @@
       <c r="G38" s="10" t="s">
         <v>403</v>
       </c>
-      <c r="H38" s="68" t="s">
-        <v>492</v>
-      </c>
+      <c r="H38" s="60"/>
     </row>
     <row r="39" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A39" s="9" t="s">
@@ -4129,9 +4325,7 @@
       <c r="G39" s="10" t="s">
         <v>403</v>
       </c>
-      <c r="H39" s="69" t="s">
-        <v>492</v>
-      </c>
+      <c r="H39" s="61"/>
     </row>
     <row r="40" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A40" s="17" t="s">
@@ -4153,9 +4347,29 @@
       <c r="G40" s="17" t="s">
         <v>403</v>
       </c>
-      <c r="H40" s="71" t="s">
-        <v>492</v>
-      </c>
+      <c r="H40" s="33"/>
+    </row>
+    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A41" s="9" t="s">
+        <v>450</v>
+      </c>
+      <c r="B41" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="C41" s="9" t="s">
+        <v>494</v>
+      </c>
+      <c r="D41" s="9"/>
+      <c r="E41" s="9" t="s">
+        <v>403</v>
+      </c>
+      <c r="F41" s="9" t="s">
+        <v>450</v>
+      </c>
+      <c r="G41" s="9" t="s">
+        <v>403</v>
+      </c>
+      <c r="H41" s="62"/>
     </row>
     <row r="43" spans="1:8" x14ac:dyDescent="0.25"/>
   </sheetData>
@@ -4166,7 +4380,7 @@
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E2:E39">
       <formula1>INDIRECT(D2)</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F2:F40">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F2:F41">
       <formula1>action_keywords</formula1>
     </dataValidation>
   </dataValidations>
@@ -4175,7 +4389,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:X9"/>
   <sheetViews>
@@ -4365,11 +4579,11 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AB36"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="T4" workbookViewId="0">
+    <sheetView showGridLines="0" workbookViewId="0">
       <selection activeCell="AB12" sqref="AB12"/>
     </sheetView>
   </sheetViews>

</xml_diff>